<commit_message>
Codigo con base de datos cargada
</commit_message>
<xml_diff>
--- a/MaterialUtil/MatrizDistancias.xlsx
+++ b/MaterialUtil/MatrizDistancias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc-I7\Desktop\TPMatematicas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Colo\TUP\Matematicas\Trabajo Practico\TP_Matematica\MaterialUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FE24742-0213-4AF6-8E2D-3D7BB00F0638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7331D9B2-08C7-46EC-8A20-271EAD594108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15600" activeTab="1" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
+    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -194,7 +194,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -255,6 +255,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -333,7 +341,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -348,13 +356,14 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -671,59 +680,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A190BE11-27A5-497D-A254-ABC1C6ECE211}">
-  <dimension ref="E6:Y28"/>
+  <dimension ref="D6:Y28"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9:D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" customWidth="1"/>
+    <col min="11" max="11" width="8.42578125" customWidth="1"/>
+    <col min="12" max="12" width="11" customWidth="1"/>
     <col min="13" max="13" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="8" customWidth="1"/>
+    <col min="16" max="16" width="6.28515625" customWidth="1"/>
+    <col min="17" max="17" width="10.7109375" customWidth="1"/>
+    <col min="18" max="18" width="7.28515625" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" customWidth="1"/>
     <col min="20" max="20" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="6.5703125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="6.85546875" customWidth="1"/>
+    <col min="23" max="23" width="7.7109375" customWidth="1"/>
     <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="5:25" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E6" s="6" t="s">
+    <row r="6" spans="4:25" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="E6" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="6"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-    </row>
-    <row r="8" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+    </row>
+    <row r="8" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
         <v>0</v>
@@ -786,7 +796,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E9" s="5" t="s">
         <v>0</v>
       </c>
@@ -851,7 +861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
@@ -916,7 +926,8 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D11" s="9"/>
       <c r="E11" s="5" t="s">
         <v>2</v>
       </c>
@@ -981,7 +992,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1046,7 +1057,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1122,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1176,7 +1187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
@@ -1241,7 +1252,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="16" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E16" s="5" t="s">
         <v>21</v>
       </c>
@@ -2099,7 +2110,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F15EB3-DAC0-4A62-AC20-08EEA7CD8347}">
   <dimension ref="E9:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
@@ -2122,13 +2133,13 @@
       <c r="E11" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="6">
         <v>3255</v>
       </c>
       <c r="H11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="I11" s="7">
+      <c r="I11" s="6">
         <v>3227</v>
       </c>
     </row>
@@ -2136,13 +2147,13 @@
       <c r="E13" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="6">
         <v>3253</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="I13" s="7">
+      <c r="I13" s="6">
         <v>3250</v>
       </c>
     </row>
@@ -2150,13 +2161,13 @@
       <c r="E15" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="6">
         <v>3276</v>
       </c>
       <c r="H15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="I15" s="7">
+      <c r="I15" s="6">
         <v>3284</v>
       </c>
     </row>
@@ -2164,13 +2175,13 @@
       <c r="E17" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>5613</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I17" s="7">
+      <c r="I17" s="6">
         <v>5462</v>
       </c>
     </row>
@@ -2178,13 +2189,13 @@
       <c r="E19" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="6">
         <v>4044</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I19" s="7">
+      <c r="I19" s="6">
         <v>4049</v>
       </c>
     </row>
@@ -2192,13 +2203,13 @@
       <c r="E21" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="6">
         <v>11491</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I21" s="6">
         <v>11487</v>
       </c>
     </row>
@@ -2206,13 +2217,13 @@
       <c r="E23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F23" s="7">
+      <c r="F23" s="6">
         <v>7785</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I23" s="7">
+      <c r="I23" s="6">
         <v>7743</v>
       </c>
     </row>
@@ -2220,13 +2231,13 @@
       <c r="E25" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F25" s="7">
+      <c r="F25" s="6">
         <v>3371</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I25" s="7">
+      <c r="I25" s="6">
         <v>3325</v>
       </c>
     </row>
@@ -2234,13 +2245,13 @@
       <c r="E27" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="F27" s="7">
+      <c r="F27" s="6">
         <v>3242</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I27" s="7">
+      <c r="I27" s="6">
         <v>3196</v>
       </c>
     </row>
@@ -2248,13 +2259,13 @@
       <c r="E29" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F29" s="7">
+      <c r="F29" s="6">
         <v>3369</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I29" s="7">
+      <c r="I29" s="6">
         <v>3208</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Partidos local y visitante en Excel
</commit_message>
<xml_diff>
--- a/MaterialUtil/MatrizDistancias.xlsx
+++ b/MaterialUtil/MatrizDistancias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Colo\TUP\Matematicas\Trabajo Practico\TP_Matematica\MaterialUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7331D9B2-08C7-46EC-8A20-271EAD594108}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E71AED-AE35-4FB3-AC8A-6E146E113A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="239">
   <si>
     <t>River Plate</t>
   </si>
@@ -130,71 +130,638 @@
     <t xml:space="preserve">Distancia total recorrida </t>
   </si>
   <si>
-    <t xml:space="preserve">Enfrentamientos </t>
-  </si>
-  <si>
-    <t>Fecha 1</t>
-  </si>
-  <si>
-    <t>Fecha 3</t>
-  </si>
-  <si>
-    <t>Fecha 4</t>
-  </si>
-  <si>
-    <t>Fecha 5</t>
-  </si>
-  <si>
-    <t>Fecha 6</t>
-  </si>
-  <si>
-    <t>Fecha 7</t>
-  </si>
-  <si>
-    <t>Fecha 8</t>
-  </si>
-  <si>
-    <t>Fecha 9</t>
-  </si>
-  <si>
-    <t>Fecha 10</t>
-  </si>
-  <si>
-    <t>Fecha 11</t>
-  </si>
-  <si>
-    <t>Fecha 12</t>
-  </si>
-  <si>
-    <t>Fecha 13</t>
-  </si>
-  <si>
-    <t>Fecha 14</t>
-  </si>
-  <si>
-    <t>Fecha 15</t>
-  </si>
-  <si>
-    <t>Fecha 16</t>
-  </si>
-  <si>
-    <t>Fecha 17</t>
-  </si>
-  <si>
-    <t>Fecha 18</t>
-  </si>
-  <si>
-    <t>Fecha 19</t>
-  </si>
-  <si>
-    <t>Fecha 2</t>
+    <t>Argentinos - banfield</t>
+  </si>
+  <si>
+    <t>belgrano - boca</t>
+  </si>
+  <si>
+    <t>colon - estudiantes</t>
+  </si>
+  <si>
+    <t>gimnasia - huracan</t>
+  </si>
+  <si>
+    <t>independiente - lanus</t>
+  </si>
+  <si>
+    <t>nob - platense</t>
+  </si>
+  <si>
+    <t>racing - river</t>
+  </si>
+  <si>
+    <t>rosario central - san lorenzo</t>
+  </si>
+  <si>
+    <t>talleres - tigre</t>
+  </si>
+  <si>
+    <t>union - velez</t>
+  </si>
+  <si>
+    <t>estudiantes - talleres</t>
+  </si>
+  <si>
+    <t>boca - racing</t>
+  </si>
+  <si>
+    <t>river - Argentinos</t>
+  </si>
+  <si>
+    <t>velez - belgrano</t>
+  </si>
+  <si>
+    <t>san lorenzo - colon</t>
+  </si>
+  <si>
+    <t>platense - independiente</t>
+  </si>
+  <si>
+    <t>huracan - rosario central</t>
+  </si>
+  <si>
+    <t>banfield - nob</t>
+  </si>
+  <si>
+    <t>lanus - union</t>
+  </si>
+  <si>
+    <t>tigre - gimnasia</t>
+  </si>
+  <si>
+    <t>talleres - platense</t>
+  </si>
+  <si>
+    <t>belgrano - estudiantes</t>
+  </si>
+  <si>
+    <t>union - huracan</t>
+  </si>
+  <si>
+    <t>rosario central - banfield</t>
+  </si>
+  <si>
+    <t>racing - lanus</t>
+  </si>
+  <si>
+    <t>nob - boca</t>
+  </si>
+  <si>
+    <t>independiente - velez</t>
+  </si>
+  <si>
+    <t>gimnasia - san lorenzo</t>
+  </si>
+  <si>
+    <t>colon - river</t>
+  </si>
+  <si>
+    <t>Argentinos - tigre</t>
+  </si>
+  <si>
+    <t>san lorenzo - talleres</t>
+  </si>
+  <si>
+    <t>boca - colon</t>
+  </si>
+  <si>
+    <t>estudiantes - independiente</t>
+  </si>
+  <si>
+    <t>platense - belgrano</t>
+  </si>
+  <si>
+    <t>huracan - nob</t>
+  </si>
+  <si>
+    <t>lanus - Argentinos</t>
+  </si>
+  <si>
+    <t>tigre - union</t>
+  </si>
+  <si>
+    <t>river - rosario central</t>
+  </si>
+  <si>
+    <t>banfield - gimnasia</t>
+  </si>
+  <si>
+    <t>velez - racing</t>
+  </si>
+  <si>
+    <t>nob - tigre</t>
+  </si>
+  <si>
+    <t>gimnasia - estudiantes</t>
+  </si>
+  <si>
+    <t>talleres - independiente</t>
+  </si>
+  <si>
+    <t>river - boca</t>
+  </si>
+  <si>
+    <t>Argentinos - platense</t>
+  </si>
+  <si>
+    <t>racing - huracan</t>
+  </si>
+  <si>
+    <t>rosario central - velez</t>
+  </si>
+  <si>
+    <t>belgrano - lanus</t>
+  </si>
+  <si>
+    <t>union - san lorenzo</t>
+  </si>
+  <si>
+    <t>colon - banfield</t>
+  </si>
+  <si>
+    <t>boca - huracan</t>
+  </si>
+  <si>
+    <t>estudiantes - rosario central</t>
+  </si>
+  <si>
+    <t>san lorenzo - velez</t>
+  </si>
+  <si>
+    <t>platense - union</t>
+  </si>
+  <si>
+    <t>independiente - belgrano</t>
+  </si>
+  <si>
+    <t>banfield - river</t>
+  </si>
+  <si>
+    <t>lanus - gimnasia</t>
+  </si>
+  <si>
+    <t>colon - nob</t>
+  </si>
+  <si>
+    <t>tigre - racing</t>
+  </si>
+  <si>
+    <t>Argentinos - talleres</t>
+  </si>
+  <si>
+    <t>VII</t>
+  </si>
+  <si>
+    <t>belgrano - colon</t>
+  </si>
+  <si>
+    <t>union - Argentinos</t>
+  </si>
+  <si>
+    <t>velez - platense</t>
+  </si>
+  <si>
+    <t>rosario central - lanus</t>
+  </si>
+  <si>
+    <t>huracan - tigre</t>
+  </si>
+  <si>
+    <t>racing - estudiantes</t>
+  </si>
+  <si>
+    <t>nob - independiente</t>
+  </si>
+  <si>
+    <t>banfield - boca</t>
+  </si>
+  <si>
+    <t>gimnasia - talleres</t>
+  </si>
+  <si>
+    <t>river - san lorenzo</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>belgrano - union</t>
+  </si>
+  <si>
+    <t>talleres - nob</t>
+  </si>
+  <si>
+    <t>estudiantes - river</t>
+  </si>
+  <si>
+    <t>san lorenzo - huracan</t>
+  </si>
+  <si>
+    <t>independiente - racing</t>
+  </si>
+  <si>
+    <t>lanus - banfield</t>
+  </si>
+  <si>
+    <t>gimnasia - boca</t>
+  </si>
+  <si>
+    <t>colon - platense</t>
+  </si>
+  <si>
+    <t>tigre - velez</t>
+  </si>
+  <si>
+    <t>Argentinos - rosario central</t>
+  </si>
+  <si>
+    <t>IX</t>
+  </si>
+  <si>
+    <t>huracan - estudiantes</t>
+  </si>
+  <si>
+    <t>boca - tigre</t>
+  </si>
+  <si>
+    <t>racing - talleres</t>
+  </si>
+  <si>
+    <t>nob - san lorenzo</t>
+  </si>
+  <si>
+    <t>river - gimnasia</t>
+  </si>
+  <si>
+    <t>velez - Argentinos</t>
+  </si>
+  <si>
+    <t>banfield - belgrano</t>
+  </si>
+  <si>
+    <t>union - colon</t>
+  </si>
+  <si>
+    <t>rosario central - independiente</t>
+  </si>
+  <si>
+    <t>platense - lanus</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>belgrano - nob</t>
+  </si>
+  <si>
+    <t>talleres - union</t>
+  </si>
+  <si>
+    <t>estudiantes - platense</t>
+  </si>
+  <si>
+    <t>san lorenzo - boca</t>
+  </si>
+  <si>
+    <t>huracan - river</t>
+  </si>
+  <si>
+    <t>independiente - colon</t>
+  </si>
+  <si>
+    <t>lanus - velez</t>
+  </si>
+  <si>
+    <t>gimnasia - rosario central</t>
+  </si>
+  <si>
+    <t>tigre - banfield</t>
+  </si>
+  <si>
+    <t>Argentinos - racing</t>
+  </si>
+  <si>
+    <t>XI</t>
+  </si>
+  <si>
+    <t>boca - estudiantes</t>
+  </si>
+  <si>
+    <t>velez - huracan</t>
+  </si>
+  <si>
+    <t>rosario central - belgrano</t>
+  </si>
+  <si>
+    <t>platense - river</t>
+  </si>
+  <si>
+    <t>racing - union</t>
+  </si>
+  <si>
+    <t>nob - gimnasia</t>
+  </si>
+  <si>
+    <t>independiente - Argentinos</t>
+  </si>
+  <si>
+    <t>banfield - san lorenzo</t>
+  </si>
+  <si>
+    <t>colon - talleres</t>
+  </si>
+  <si>
+    <t>tigre - lanus</t>
+  </si>
+  <si>
+    <t>XII</t>
+  </si>
+  <si>
+    <t>boca - rosario central</t>
+  </si>
+  <si>
+    <t>union - independiente</t>
+  </si>
+  <si>
+    <t>talleres - belgrano</t>
+  </si>
+  <si>
+    <t>estudiantes - nob</t>
+  </si>
+  <si>
+    <t>san lorenzo - lanus</t>
+  </si>
+  <si>
+    <t>huracan - banfield</t>
+  </si>
+  <si>
+    <t>racing - platense</t>
+  </si>
+  <si>
+    <t>gimnasia - velez</t>
+  </si>
+  <si>
+    <t>Argentinos - colon</t>
+  </si>
+  <si>
+    <t>river - tigre</t>
+  </si>
+  <si>
+    <t>XIII</t>
+  </si>
+  <si>
+    <t>belgrano - Argentinos</t>
+  </si>
+  <si>
+    <t>velez - banfield</t>
+  </si>
+  <si>
+    <t>talleres - river</t>
+  </si>
+  <si>
+    <t>estudiantes - union</t>
+  </si>
+  <si>
+    <t>platense - boca</t>
+  </si>
+  <si>
+    <t>nob - racing</t>
+  </si>
+  <si>
+    <t>independiente - san lorenzo</t>
+  </si>
+  <si>
+    <t>lanus - huracan</t>
+  </si>
+  <si>
+    <t>colon - gimnasia</t>
+  </si>
+  <si>
+    <t>tigre - rosario central</t>
+  </si>
+  <si>
+    <t>XIV</t>
+  </si>
+  <si>
+    <t>boca - velez</t>
+  </si>
+  <si>
+    <t>union - nob</t>
+  </si>
+  <si>
+    <t>rosario central - platense</t>
+  </si>
+  <si>
+    <t>san lorenzo - tigre</t>
+  </si>
+  <si>
+    <t>huracan - talleres</t>
+  </si>
+  <si>
+    <t>racing - colon</t>
+  </si>
+  <si>
+    <t>banfield - independiente</t>
+  </si>
+  <si>
+    <t>gimnasia - belgrano</t>
+  </si>
+  <si>
+    <t>Argentinos - estudiantes</t>
+  </si>
+  <si>
+    <t>river - lanus</t>
+  </si>
+  <si>
+    <t>XV</t>
+  </si>
+  <si>
+    <t>belgrano - racing</t>
+  </si>
+  <si>
+    <t>lanus - boca</t>
+  </si>
+  <si>
+    <t>independiente - huracan</t>
+  </si>
+  <si>
+    <t>nob - Argentinos</t>
+  </si>
+  <si>
+    <t>platense - gimnasia</t>
+  </si>
+  <si>
+    <t>estudiantes - san lorenzo</t>
+  </si>
+  <si>
+    <t>talleres - rosario central</t>
+  </si>
+  <si>
+    <t>velez - river</t>
+  </si>
+  <si>
+    <t>union - banfield</t>
+  </si>
+  <si>
+    <t>colon - tigre</t>
+  </si>
+  <si>
+    <t>XVI</t>
+  </si>
+  <si>
+    <t>boca - Argentinos</t>
+  </si>
+  <si>
+    <t>velez - estudiantes</t>
+  </si>
+  <si>
+    <t>rosario central - nob</t>
+  </si>
+  <si>
+    <t>san lorenzo - racing</t>
+  </si>
+  <si>
+    <t>huracan - platense</t>
+  </si>
+  <si>
+    <t>banfield - talleres</t>
+  </si>
+  <si>
+    <t>lanus - colon</t>
+  </si>
+  <si>
+    <t>gimnasia - independiente</t>
+  </si>
+  <si>
+    <t>tigre - belgrano</t>
+  </si>
+  <si>
+    <t>river - union</t>
+  </si>
+  <si>
+    <t>XVII</t>
+  </si>
+  <si>
+    <t>belgrano - river</t>
+  </si>
+  <si>
+    <t>union - rosario central</t>
+  </si>
+  <si>
+    <t>talleres - lanus</t>
+  </si>
+  <si>
+    <t>estudiantes - tigre</t>
+  </si>
+  <si>
+    <t>platense - san lorenzo</t>
+  </si>
+  <si>
+    <t>racing - banfield</t>
+  </si>
+  <si>
+    <t>nob - velez</t>
+  </si>
+  <si>
+    <t>independiente - boca</t>
+  </si>
+  <si>
+    <t>colon - huracan</t>
+  </si>
+  <si>
+    <t>Argentinos - gimnasia</t>
+  </si>
+  <si>
+    <t>XVIII</t>
+  </si>
+  <si>
+    <t>boca - talleres</t>
+  </si>
+  <si>
+    <t>velez - colon</t>
+  </si>
+  <si>
+    <t>rosario central - racing</t>
+  </si>
+  <si>
+    <t>san lorenzo - belgrano</t>
+  </si>
+  <si>
+    <t>huracan - Argentinos</t>
+  </si>
+  <si>
+    <t>banfield - platense</t>
+  </si>
+  <si>
+    <t>lanus - estudiantes</t>
+  </si>
+  <si>
+    <t>gimnasia - union</t>
+  </si>
+  <si>
+    <t>tigre - independiente</t>
+  </si>
+  <si>
+    <t>river - nob</t>
+  </si>
+  <si>
+    <t>XIX</t>
+  </si>
+  <si>
+    <t>Argentinos - san lorenzo</t>
+  </si>
+  <si>
+    <t>union - boca</t>
+  </si>
+  <si>
+    <t>talleres - velez</t>
+  </si>
+  <si>
+    <t>estudiantes - banfield</t>
+  </si>
+  <si>
+    <t>platense - tigre</t>
+  </si>
+  <si>
+    <t>racing - gimnasia</t>
+  </si>
+  <si>
+    <t>nob - lanus</t>
+  </si>
+  <si>
+    <t>independiente - river</t>
+  </si>
+  <si>
+    <t>colon - rosario central</t>
+  </si>
+  <si>
+    <t>belgrano - huracan</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>IV</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>VI</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -267,8 +834,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,6 +877,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -341,7 +941,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -357,13 +957,31 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -682,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A190BE11-27A5-497D-A254-ABC1C6ECE211}">
   <dimension ref="D6:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9:E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -709,29 +1327,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:25" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
     </row>
     <row r="8" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
@@ -927,7 +1545,7 @@
       </c>
     </row>
     <row r="11" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D11" s="9"/>
+      <c r="D11" s="7"/>
       <c r="E11" s="5" t="s">
         <v>2</v>
       </c>
@@ -2121,13 +2739,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="E9" s="8" t="s">
+      <c r="E9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9"/>
     </row>
     <row r="11" spans="5:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
@@ -2280,116 +2898,721 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2B0C72-7996-4F05-A4C8-44CF30165835}">
-  <dimension ref="C8:C28"/>
+  <dimension ref="B9:X114"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K24" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="11" width="27.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C8" t="s">
+    <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="13" t="s">
+        <v>233</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>235</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>237</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="12" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="H10" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="K10" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="R10" s="10"/>
+      <c r="T10" s="10"/>
+      <c r="V10" s="10"/>
+    </row>
+    <row r="11" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="12" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="C11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>103</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="K11" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="X11" s="10"/>
+    </row>
+    <row r="12" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>85</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="J15" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>87</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>99</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="12" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
-        <v>48</v>
-      </c>
+      <c r="D19" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="11"/>
+      <c r="K20" s="11"/>
+    </row>
+    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="E21" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="F21" s="13" t="s">
+        <v>178</v>
+      </c>
+      <c r="G21" s="13" t="s">
+        <v>189</v>
+      </c>
+      <c r="H21" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="K21" s="11"/>
+    </row>
+    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="C22" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="F22" s="12" t="s">
+        <v>179</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="I22" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="J22" s="12" t="s">
+        <v>223</v>
+      </c>
+      <c r="K22" s="11"/>
+    </row>
+    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="12" t="s">
+        <v>136</v>
+      </c>
+      <c r="C23" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="F23" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="I23" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>224</v>
+      </c>
+      <c r="K23" s="11"/>
+    </row>
+    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="12" t="s">
+        <v>137</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="F24" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="G24" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H24" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="I24" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="J24" s="12" t="s">
+        <v>225</v>
+      </c>
+      <c r="K24" s="15"/>
+    </row>
+    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="12" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="D25" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="H25" s="12" t="s">
+        <v>204</v>
+      </c>
+      <c r="I25" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>226</v>
+      </c>
+      <c r="K25" s="11"/>
+    </row>
+    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="H26" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="I26" s="12" t="s">
+        <v>216</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>227</v>
+      </c>
+      <c r="K26" s="11"/>
+    </row>
+    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="12" t="s">
+        <v>140</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="H27" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>217</v>
+      </c>
+      <c r="J27" s="12" t="s">
+        <v>228</v>
+      </c>
+      <c r="K27" s="11"/>
+    </row>
+    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="C28" s="12" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="H28" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="I28" s="12" t="s">
+        <v>218</v>
+      </c>
+      <c r="J28" s="12" t="s">
+        <v>229</v>
+      </c>
+      <c r="K28" s="11"/>
+    </row>
+    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="H29" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="I29" s="12" t="s">
+        <v>219</v>
+      </c>
+      <c r="J29" s="12" t="s">
+        <v>230</v>
+      </c>
+      <c r="K29" s="11"/>
+    </row>
+    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="C30" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>198</v>
+      </c>
+      <c r="H30" s="12" t="s">
+        <v>209</v>
+      </c>
+      <c r="I30" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="J30" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="K30" s="11"/>
+    </row>
+    <row r="31" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C31" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="H31" s="12" t="s">
+        <v>210</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>221</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>232</v>
+      </c>
+      <c r="K31" s="11"/>
+    </row>
+    <row r="114" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K114" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lista de tareas a dividir
</commit_message>
<xml_diff>
--- a/MaterialUtil/MatrizDistancias.xlsx
+++ b/MaterialUtil/MatrizDistancias.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Colo\TUP\Matematicas\Trabajo Practico\TP_Matematica\MaterialUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E71AED-AE35-4FB3-AC8A-6E146E113A7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5B7C69-2658-4202-B0BA-6CF97F3BEF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="249">
   <si>
     <t>River Plate</t>
   </si>
@@ -755,6 +755,36 @@
   </si>
   <si>
     <t>VI</t>
+  </si>
+  <si>
+    <t>17-14</t>
+  </si>
+  <si>
+    <t>11--01</t>
+  </si>
+  <si>
+    <t>12--8</t>
+  </si>
+  <si>
+    <t>9--5</t>
+  </si>
+  <si>
+    <t>2--15</t>
+  </si>
+  <si>
+    <t>7--19</t>
+  </si>
+  <si>
+    <t>3--0</t>
+  </si>
+  <si>
+    <t>6--4</t>
+  </si>
+  <si>
+    <t>10--18</t>
+  </si>
+  <si>
+    <t>13--16</t>
   </si>
 </sst>
 </file>
@@ -941,7 +971,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -958,12 +988,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -981,6 +1005,24 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1300,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A190BE11-27A5-497D-A254-ABC1C6ECE211}">
   <dimension ref="D6:Y28"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9:E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1323,33 +1365,33 @@
     <col min="22" max="22" width="6.85546875" customWidth="1"/>
     <col min="23" max="23" width="7.7109375" customWidth="1"/>
     <col min="24" max="24" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4.5703125" customWidth="1"/>
+    <col min="25" max="25" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="4:25" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="8"/>
-      <c r="O6" s="8"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="8"/>
-      <c r="S6" s="8"/>
-      <c r="T6" s="8"/>
-      <c r="U6" s="8"/>
-      <c r="V6" s="8"/>
-      <c r="W6" s="8"/>
-      <c r="X6" s="8"/>
-      <c r="Y6" s="8"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+      <c r="N6" s="14"/>
+      <c r="O6" s="14"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="14"/>
+      <c r="S6" s="14"/>
+      <c r="T6" s="14"/>
+      <c r="U6" s="14"/>
+      <c r="V6" s="14"/>
+      <c r="W6" s="14"/>
+      <c r="X6" s="14"/>
+      <c r="Y6" s="14"/>
     </row>
     <row r="8" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
@@ -1415,6 +1457,9 @@
       </c>
     </row>
     <row r="9" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D9">
+        <v>0</v>
+      </c>
       <c r="E9" s="5" t="s">
         <v>0</v>
       </c>
@@ -1480,6 +1525,9 @@
       </c>
     </row>
     <row r="10" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D10">
+        <v>1</v>
+      </c>
       <c r="E10" s="5" t="s">
         <v>1</v>
       </c>
@@ -1545,7 +1593,9 @@
       </c>
     </row>
     <row r="11" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D11" s="7"/>
+      <c r="D11" s="7">
+        <v>2</v>
+      </c>
       <c r="E11" s="5" t="s">
         <v>2</v>
       </c>
@@ -1611,6 +1661,9 @@
       </c>
     </row>
     <row r="12" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>3</v>
+      </c>
       <c r="E12" s="5" t="s">
         <v>3</v>
       </c>
@@ -1676,6 +1729,9 @@
       </c>
     </row>
     <row r="13" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D13">
+        <v>4</v>
+      </c>
       <c r="E13" s="5" t="s">
         <v>4</v>
       </c>
@@ -1741,6 +1797,9 @@
       </c>
     </row>
     <row r="14" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D14">
+        <v>5</v>
+      </c>
       <c r="E14" s="5" t="s">
         <v>5</v>
       </c>
@@ -1806,6 +1865,9 @@
       </c>
     </row>
     <row r="15" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D15" s="7">
+        <v>6</v>
+      </c>
       <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
@@ -1871,6 +1933,9 @@
       </c>
     </row>
     <row r="16" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D16">
+        <v>7</v>
+      </c>
       <c r="E16" s="5" t="s">
         <v>21</v>
       </c>
@@ -1935,7 +2000,10 @@
         <v>284</v>
       </c>
     </row>
-    <row r="17" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D17">
+        <v>8</v>
+      </c>
       <c r="E17" s="5" t="s">
         <v>7</v>
       </c>
@@ -2000,7 +2068,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="18" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D18">
+        <v>9</v>
+      </c>
       <c r="E18" s="5" t="s">
         <v>8</v>
       </c>
@@ -2065,7 +2136,10 @@
         <v>71</v>
       </c>
     </row>
-    <row r="19" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D19" s="7">
+        <v>10</v>
+      </c>
       <c r="E19" s="5" t="s">
         <v>9</v>
       </c>
@@ -2130,7 +2204,10 @@
         <v>683</v>
       </c>
     </row>
-    <row r="20" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>11</v>
+      </c>
       <c r="E20" s="5" t="s">
         <v>10</v>
       </c>
@@ -2195,7 +2272,10 @@
         <v>685</v>
       </c>
     </row>
-    <row r="21" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <v>12</v>
+      </c>
       <c r="E21" s="5" t="s">
         <v>11</v>
       </c>
@@ -2260,7 +2340,10 @@
         <v>455</v>
       </c>
     </row>
-    <row r="22" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <v>13</v>
+      </c>
       <c r="E22" s="5" t="s">
         <v>12</v>
       </c>
@@ -2325,7 +2408,10 @@
         <v>451</v>
       </c>
     </row>
-    <row r="23" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D23" s="7">
+        <v>14</v>
+      </c>
       <c r="E23" s="5" t="s">
         <v>13</v>
       </c>
@@ -2390,7 +2476,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="24" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D24">
+        <v>15</v>
+      </c>
       <c r="E24" s="5" t="s">
         <v>14</v>
       </c>
@@ -2455,7 +2544,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D25">
+        <v>16</v>
+      </c>
       <c r="E25" s="5" t="s">
         <v>15</v>
       </c>
@@ -2520,7 +2612,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="26" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D26">
+        <v>17</v>
+      </c>
       <c r="E26" s="5" t="s">
         <v>16</v>
       </c>
@@ -2585,7 +2680,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D27" s="7">
+        <v>18</v>
+      </c>
       <c r="E27" s="5" t="s">
         <v>17</v>
       </c>
@@ -2650,7 +2748,10 @@
         <v>16</v>
       </c>
     </row>
-    <row r="28" spans="5:25" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D28">
+        <v>19</v>
+      </c>
       <c r="E28" s="5" t="s">
         <v>18</v>
       </c>
@@ -2739,13 +2840,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
     </row>
     <row r="11" spans="5:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
@@ -2898,717 +2999,1086 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2B0C72-7996-4F05-A4C8-44CF30165835}">
-  <dimension ref="B9:X114"/>
+  <dimension ref="A9:AH114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K24" sqref="K24"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="topRight" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="11" width="27.7109375" customWidth="1"/>
+    <col min="2" max="2" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" customWidth="1"/>
+    <col min="9" max="9" width="27.7109375" customWidth="1"/>
+    <col min="10" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="27.7109375" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" customWidth="1"/>
+    <col min="13" max="13" width="27.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
+    <col min="15" max="15" width="27.7109375" customWidth="1"/>
+    <col min="16" max="16" width="8.7109375" customWidth="1"/>
+    <col min="17" max="17" width="27.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="27.7109375" customWidth="1"/>
+    <col min="20" max="20" width="8.7109375" customWidth="1"/>
+    <col min="21" max="21" width="27.7109375" customWidth="1"/>
+    <col min="24" max="24" width="33.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="9" spans="2:24" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B9" s="13" t="s">
+    <row r="9" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="C9" s="11" t="s">
         <v>233</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="D9" s="11"/>
+      <c r="E9" s="12" t="s">
         <v>235</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="F9" s="12"/>
+      <c r="G9" s="12" t="s">
         <v>234</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="H9" s="12"/>
+      <c r="I9" s="12" t="s">
         <v>236</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="J9" s="12"/>
+      <c r="K9" s="12" t="s">
         <v>237</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="L9" s="12"/>
+      <c r="M9" s="12" t="s">
         <v>238</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="N9" s="12"/>
+      <c r="O9" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="P9" s="12"/>
+      <c r="Q9" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="R9" s="12"/>
+      <c r="S9" s="12" t="s">
         <v>112</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="T9" s="12"/>
+      <c r="U9" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+    <row r="10" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="D10" s="10" t="s">
+        <v>239</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="F10" s="10"/>
+      <c r="G10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="E10" s="12" t="s">
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="J10" s="10"/>
+      <c r="K10" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="L10" s="10"/>
+      <c r="M10" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="H10" s="12" t="s">
+      <c r="N10" s="10"/>
+      <c r="O10" s="10" t="s">
         <v>91</v>
       </c>
-      <c r="I10" s="12" t="s">
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="J10" s="12" t="s">
+      <c r="R10" s="10"/>
+      <c r="S10" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="K10" s="12" t="s">
+      <c r="T10" s="10"/>
+      <c r="U10" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="R10" s="10"/>
-      <c r="T10" s="10"/>
-      <c r="V10" s="10"/>
-    </row>
-    <row r="11" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="12" t="s">
+      <c r="AB10" s="8"/>
+      <c r="AD10" s="8"/>
+      <c r="AF10" s="8"/>
+    </row>
+    <row r="11" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="D11" s="18" t="s">
+        <v>240</v>
+      </c>
+      <c r="E11" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="F11" s="10"/>
+      <c r="G11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="12" t="s">
+      <c r="H11" s="10"/>
+      <c r="I11" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="12" t="s">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="L11" s="10"/>
+      <c r="M11" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="H11" s="12" t="s">
+      <c r="N11" s="10"/>
+      <c r="O11" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="J11" s="12" t="s">
+      <c r="R11" s="10"/>
+      <c r="S11" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="K11" s="12" t="s">
+      <c r="T11" s="10"/>
+      <c r="U11" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="X11" s="10"/>
-    </row>
-    <row r="12" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="12" t="s">
+      <c r="AH11" s="8"/>
+    </row>
+    <row r="12" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>2</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="10" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E12" s="12" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="L12" s="10"/>
+      <c r="M12" s="10" t="s">
         <v>82</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="N12" s="10"/>
+      <c r="O12" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="I12" s="12" t="s">
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="J12" s="12" t="s">
+      <c r="R12" s="10"/>
+      <c r="S12" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="K12" s="12" t="s">
+      <c r="T12" s="10"/>
+      <c r="U12" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12" t="s">
+    <row r="13" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="D13" s="10" t="s">
+        <v>242</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="F13" s="10"/>
+      <c r="G13" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="12" t="s">
+      <c r="H13" s="10"/>
+      <c r="I13" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="J13" s="10"/>
+      <c r="K13" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="L13" s="10"/>
+      <c r="M13" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="H13" s="12" t="s">
+      <c r="N13" s="10"/>
+      <c r="O13" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="I13" s="12" t="s">
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="J13" s="12" t="s">
+      <c r="R13" s="10"/>
+      <c r="S13" s="10" t="s">
         <v>116</v>
       </c>
-      <c r="K13" s="12" t="s">
+      <c r="T13" s="10"/>
+      <c r="U13" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
+    <row r="14" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="D14" s="19" t="s">
+        <v>243</v>
+      </c>
+      <c r="E14" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="F14" s="10"/>
+      <c r="G14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E14" s="12" t="s">
+      <c r="H14" s="10"/>
+      <c r="I14" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="J14" s="10"/>
+      <c r="K14" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="L14" s="10"/>
+      <c r="M14" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="N14" s="10"/>
+      <c r="O14" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="I14" s="12" t="s">
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="J14" s="12" t="s">
+      <c r="R14" s="10"/>
+      <c r="S14" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="T14" s="10"/>
+      <c r="U14" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
+    <row r="15" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="D15" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="E15" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="F15" s="10"/>
+      <c r="G15" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="12" t="s">
+      <c r="H15" s="10"/>
+      <c r="I15" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="F15" s="12" t="s">
+      <c r="J15" s="10"/>
+      <c r="K15" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="L15" s="10"/>
+      <c r="M15" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="H15" s="12" t="s">
+      <c r="N15" s="10"/>
+      <c r="O15" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="I15" s="12" t="s">
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="J15" s="12" t="s">
+      <c r="R15" s="10"/>
+      <c r="S15" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="K15" s="12" t="s">
+      <c r="T15" s="10"/>
+      <c r="U15" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="2:24" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
+    <row r="16" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>6</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="D16" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="E16" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="F16" s="10"/>
+      <c r="G16" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="H16" s="10"/>
+      <c r="I16" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="12" t="s">
+      <c r="J16" s="10"/>
+      <c r="K16" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="L16" s="10"/>
+      <c r="M16" s="10" t="s">
         <v>86</v>
       </c>
-      <c r="H16" s="12" t="s">
+      <c r="N16" s="10"/>
+      <c r="O16" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="I16" s="12" t="s">
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="12" t="s">
+      <c r="R16" s="10"/>
+      <c r="S16" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="K16" s="12" t="s">
+      <c r="T16" s="10"/>
+      <c r="U16" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="17" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
+    <row r="17" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="D17" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="E17" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="F17" s="10"/>
+      <c r="G17" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="12" t="s">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="12" t="s">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="L17" s="10"/>
+      <c r="M17" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="N17" s="10"/>
+      <c r="O17" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="I17" s="12" t="s">
+      <c r="P17" s="10"/>
+      <c r="Q17" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="J17" s="12" t="s">
+      <c r="R17" s="10"/>
+      <c r="S17" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="K17" s="12" t="s">
+      <c r="T17" s="10"/>
+      <c r="U17" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="18" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
+    <row r="18" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="D18" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="F18" s="10"/>
+      <c r="G18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="H18" s="10"/>
+      <c r="I18" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="12" t="s">
+      <c r="J18" s="10"/>
+      <c r="K18" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="L18" s="10"/>
+      <c r="M18" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="N18" s="10"/>
+      <c r="O18" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="I18" s="12" t="s">
+      <c r="P18" s="10"/>
+      <c r="Q18" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="J18" s="12" t="s">
+      <c r="R18" s="10"/>
+      <c r="S18" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="K18" s="12" t="s">
+      <c r="T18" s="10"/>
+      <c r="U18" s="10" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="19" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="12" t="s">
+    <row r="19" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="D19" s="10" t="s">
+        <v>248</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="F19" s="10"/>
+      <c r="G19" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="H19" s="10"/>
+      <c r="I19" s="10" t="s">
         <v>69</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="J19" s="10"/>
+      <c r="K19" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="H19" s="12" t="s">
+      <c r="N19" s="10"/>
+      <c r="O19" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="I19" s="12" t="s">
+      <c r="P19" s="10"/>
+      <c r="Q19" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="J19" s="12" t="s">
+      <c r="R19" s="10"/>
+      <c r="S19" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="T19" s="10"/>
+      <c r="U19" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-    </row>
-    <row r="21" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="13" t="s">
+    <row r="20" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="7">
+        <v>10</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="13"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+    </row>
+    <row r="21" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="D21" s="11"/>
+      <c r="E21" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="F21" s="11"/>
+      <c r="G21" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="H21" s="11"/>
+      <c r="I21" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="J21" s="11"/>
+      <c r="K21" s="11" t="s">
         <v>178</v>
       </c>
-      <c r="G21" s="13" t="s">
+      <c r="L21" s="11"/>
+      <c r="M21" s="11" t="s">
         <v>189</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="N21" s="11"/>
+      <c r="O21" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="I21" s="13" t="s">
+      <c r="P21" s="11"/>
+      <c r="Q21" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="R21" s="11"/>
+      <c r="S21" s="11" t="s">
         <v>222</v>
       </c>
-      <c r="K21" s="11"/>
-    </row>
-    <row r="22" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="12" t="s">
+      <c r="T21" s="16"/>
+      <c r="U21" s="9"/>
+    </row>
+    <row r="22" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="D22" s="10"/>
+      <c r="E22" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="F22" s="10"/>
+      <c r="G22" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="E22" s="12" t="s">
+      <c r="H22" s="10"/>
+      <c r="I22" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="J22" s="10"/>
+      <c r="K22" s="10" t="s">
         <v>179</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="L22" s="10"/>
+      <c r="M22" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="H22" s="12" t="s">
+      <c r="N22" s="10"/>
+      <c r="O22" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="P22" s="10"/>
+      <c r="Q22" s="10" t="s">
         <v>212</v>
       </c>
-      <c r="J22" s="12" t="s">
+      <c r="R22" s="10"/>
+      <c r="S22" s="10" t="s">
         <v>223</v>
       </c>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="12" t="s">
+      <c r="T22" s="17"/>
+      <c r="U22" s="9"/>
+    </row>
+    <row r="23" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="10" t="s">
         <v>136</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="D23" s="10"/>
+      <c r="E23" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="F23" s="10"/>
+      <c r="G23" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="E23" s="12" t="s">
+      <c r="H23" s="10"/>
+      <c r="I23" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="J23" s="10"/>
+      <c r="K23" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="L23" s="10"/>
+      <c r="M23" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="H23" s="12" t="s">
+      <c r="N23" s="10"/>
+      <c r="O23" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="I23" s="12" t="s">
+      <c r="P23" s="10"/>
+      <c r="Q23" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="J23" s="12" t="s">
+      <c r="R23" s="10"/>
+      <c r="S23" s="10" t="s">
         <v>224</v>
       </c>
-      <c r="K23" s="11"/>
-    </row>
-    <row r="24" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="12" t="s">
+      <c r="T23" s="17"/>
+      <c r="U23" s="9"/>
+    </row>
+    <row r="24" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>14</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="10" t="s">
         <v>137</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="D24" s="10"/>
+      <c r="E24" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="F24" s="10"/>
+      <c r="G24" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="E24" s="12" t="s">
+      <c r="H24" s="10"/>
+      <c r="I24" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="F24" s="12" t="s">
+      <c r="J24" s="10"/>
+      <c r="K24" s="10" t="s">
         <v>181</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="L24" s="10"/>
+      <c r="M24" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="H24" s="12" t="s">
+      <c r="N24" s="10"/>
+      <c r="O24" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="I24" s="12" t="s">
+      <c r="P24" s="10"/>
+      <c r="Q24" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="J24" s="12" t="s">
+      <c r="R24" s="10"/>
+      <c r="S24" s="10" t="s">
         <v>225</v>
       </c>
-      <c r="K24" s="15"/>
-    </row>
-    <row r="25" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="12" t="s">
+      <c r="T24" s="17"/>
+      <c r="U24" s="13"/>
+    </row>
+    <row r="25" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C25" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="D25" s="10"/>
+      <c r="E25" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="F25" s="10"/>
+      <c r="G25" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="E25" s="12" t="s">
+      <c r="H25" s="10"/>
+      <c r="I25" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="F25" s="12" t="s">
+      <c r="J25" s="10"/>
+      <c r="K25" s="10" t="s">
         <v>182</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="L25" s="10"/>
+      <c r="M25" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="H25" s="12" t="s">
+      <c r="N25" s="10"/>
+      <c r="O25" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="I25" s="12" t="s">
+      <c r="P25" s="10"/>
+      <c r="Q25" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="J25" s="12" t="s">
+      <c r="R25" s="10"/>
+      <c r="S25" s="10" t="s">
         <v>226</v>
       </c>
-      <c r="K25" s="11"/>
-    </row>
-    <row r="26" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
+      <c r="T25" s="17"/>
+      <c r="U25" s="9"/>
+    </row>
+    <row r="26" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="D26" s="10"/>
+      <c r="E26" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="F26" s="10"/>
+      <c r="G26" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="E26" s="12" t="s">
+      <c r="H26" s="10"/>
+      <c r="I26" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="F26" s="12" t="s">
+      <c r="J26" s="10"/>
+      <c r="K26" s="10" t="s">
         <v>183</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="L26" s="10"/>
+      <c r="M26" s="10" t="s">
         <v>194</v>
       </c>
-      <c r="H26" s="12" t="s">
+      <c r="N26" s="10"/>
+      <c r="O26" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="I26" s="12" t="s">
+      <c r="P26" s="10"/>
+      <c r="Q26" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="J26" s="12" t="s">
+      <c r="R26" s="10"/>
+      <c r="S26" s="10" t="s">
         <v>227</v>
       </c>
-      <c r="K26" s="11"/>
-    </row>
-    <row r="27" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12" t="s">
+      <c r="T26" s="17"/>
+      <c r="U26" s="9"/>
+    </row>
+    <row r="27" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="D27" s="10"/>
+      <c r="E27" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="F27" s="10"/>
+      <c r="G27" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="E27" s="12" t="s">
+      <c r="H27" s="10"/>
+      <c r="I27" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="F27" s="12" t="s">
+      <c r="J27" s="10"/>
+      <c r="K27" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="G27" s="12" t="s">
+      <c r="L27" s="10"/>
+      <c r="M27" s="10" t="s">
         <v>195</v>
       </c>
-      <c r="H27" s="12" t="s">
+      <c r="N27" s="10"/>
+      <c r="O27" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="12" t="s">
+      <c r="P27" s="10"/>
+      <c r="Q27" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="J27" s="12" t="s">
+      <c r="R27" s="10"/>
+      <c r="S27" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="K27" s="11"/>
-    </row>
-    <row r="28" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="12" t="s">
+      <c r="T27" s="17"/>
+      <c r="U27" s="9"/>
+    </row>
+    <row r="28" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="7">
+        <v>18</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>141</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="D28" s="10"/>
+      <c r="E28" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="E28" s="12" t="s">
+      <c r="H28" s="10"/>
+      <c r="I28" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="F28" s="12" t="s">
+      <c r="J28" s="10"/>
+      <c r="K28" s="10" t="s">
         <v>185</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="L28" s="10"/>
+      <c r="M28" s="10" t="s">
         <v>196</v>
       </c>
-      <c r="H28" s="12" t="s">
+      <c r="N28" s="10"/>
+      <c r="O28" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="I28" s="12" t="s">
+      <c r="P28" s="10"/>
+      <c r="Q28" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="J28" s="12" t="s">
+      <c r="R28" s="10"/>
+      <c r="S28" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="K28" s="11"/>
-    </row>
-    <row r="29" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="12" t="s">
+      <c r="T28" s="17"/>
+      <c r="U28" s="9"/>
+    </row>
+    <row r="29" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="D29" s="10"/>
+      <c r="E29" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="F29" s="10"/>
+      <c r="G29" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="E29" s="12" t="s">
+      <c r="H29" s="10"/>
+      <c r="I29" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="F29" s="12" t="s">
+      <c r="J29" s="10"/>
+      <c r="K29" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="G29" s="12" t="s">
+      <c r="L29" s="10"/>
+      <c r="M29" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H29" s="12" t="s">
+      <c r="N29" s="10"/>
+      <c r="O29" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="P29" s="10"/>
+      <c r="Q29" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="J29" s="12" t="s">
+      <c r="R29" s="10"/>
+      <c r="S29" s="10" t="s">
         <v>230</v>
       </c>
-      <c r="K29" s="11"/>
-    </row>
-    <row r="30" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+      <c r="T29" s="17"/>
+      <c r="U29" s="9"/>
+    </row>
+    <row r="30" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C30" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="D30" s="10"/>
+      <c r="E30" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="F30" s="10"/>
+      <c r="G30" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E30" s="12" t="s">
+      <c r="H30" s="10"/>
+      <c r="I30" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="F30" s="12" t="s">
+      <c r="J30" s="10"/>
+      <c r="K30" s="10" t="s">
         <v>187</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="L30" s="10"/>
+      <c r="M30" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="H30" s="12" t="s">
+      <c r="N30" s="10"/>
+      <c r="O30" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="P30" s="10"/>
+      <c r="Q30" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="J30" s="12" t="s">
+      <c r="R30" s="10"/>
+      <c r="S30" s="10" t="s">
         <v>231</v>
       </c>
-      <c r="K30" s="11"/>
-    </row>
-    <row r="31" spans="2:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+      <c r="T30" s="17"/>
+      <c r="U30" s="9"/>
+    </row>
+    <row r="31" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C31" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="D31" s="10"/>
+      <c r="E31" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="F31" s="10"/>
+      <c r="G31" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="E31" s="12" t="s">
+      <c r="H31" s="10"/>
+      <c r="I31" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="J31" s="10"/>
+      <c r="K31" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="L31" s="10"/>
+      <c r="M31" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="H31" s="12" t="s">
+      <c r="N31" s="10"/>
+      <c r="O31" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="P31" s="10"/>
+      <c r="Q31" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="J31" s="12" t="s">
+      <c r="R31" s="10"/>
+      <c r="S31" s="10" t="s">
         <v>232</v>
       </c>
-      <c r="K31" s="11"/>
-    </row>
-    <row r="114" spans="11:11" x14ac:dyDescent="0.25">
-      <c r="K114" s="7"/>
+      <c r="T31" s="17"/>
+      <c r="U31" s="9"/>
+    </row>
+    <row r="114" spans="21:21" x14ac:dyDescent="0.25">
+      <c r="U114" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>

</xml_diff>

<commit_message>
Clasico en fecha 7
</commit_message>
<xml_diff>
--- a/MaterialUtil/MatrizDistancias.xlsx
+++ b/MaterialUtil/MatrizDistancias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Colo\TUP\Matematicas\Trabajo Practico\TP_Matematica\MaterialUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E5B7C69-2658-4202-B0BA-6CF97F3BEF5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B58EE49-7FD7-48EB-BE29-DED513AEE1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -145,9 +145,6 @@
     <t>independiente - lanus</t>
   </si>
   <si>
-    <t>nob - platense</t>
-  </si>
-  <si>
     <t>racing - river</t>
   </si>
   <si>
@@ -181,9 +178,6 @@
     <t>huracan - rosario central</t>
   </si>
   <si>
-    <t>banfield - nob</t>
-  </si>
-  <si>
     <t>lanus - union</t>
   </si>
   <si>
@@ -205,9 +199,6 @@
     <t>racing - lanus</t>
   </si>
   <si>
-    <t>nob - boca</t>
-  </si>
-  <si>
     <t>independiente - velez</t>
   </si>
   <si>
@@ -232,9 +223,6 @@
     <t>platense - belgrano</t>
   </si>
   <si>
-    <t>huracan - nob</t>
-  </si>
-  <si>
     <t>lanus - Argentinos</t>
   </si>
   <si>
@@ -250,9 +238,6 @@
     <t>velez - racing</t>
   </si>
   <si>
-    <t>nob - tigre</t>
-  </si>
-  <si>
     <t>gimnasia - estudiantes</t>
   </si>
   <si>
@@ -301,9 +286,6 @@
     <t>lanus - gimnasia</t>
   </si>
   <si>
-    <t>colon - nob</t>
-  </si>
-  <si>
     <t>tigre - racing</t>
   </si>
   <si>
@@ -349,9 +331,6 @@
     <t>belgrano - union</t>
   </si>
   <si>
-    <t>talleres - nob</t>
-  </si>
-  <si>
     <t>estudiantes - river</t>
   </si>
   <si>
@@ -388,9 +367,6 @@
     <t>racing - talleres</t>
   </si>
   <si>
-    <t>nob - san lorenzo</t>
-  </si>
-  <si>
     <t>river - gimnasia</t>
   </si>
   <si>
@@ -412,9 +388,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>belgrano - nob</t>
-  </si>
-  <si>
     <t>talleres - union</t>
   </si>
   <si>
@@ -785,13 +758,40 @@
   </si>
   <si>
     <t>13--16</t>
+  </si>
+  <si>
+    <t>platense - nob</t>
+  </si>
+  <si>
+    <t>nob - banfield</t>
+  </si>
+  <si>
+    <t>boca - nob</t>
+  </si>
+  <si>
+    <t>nob - huracan</t>
+  </si>
+  <si>
+    <t>tigre - nob</t>
+  </si>
+  <si>
+    <t>nob - colon</t>
+  </si>
+  <si>
+    <t>nob - talleres</t>
+  </si>
+  <si>
+    <t>san lo renzo - nob</t>
+  </si>
+  <si>
+    <t>nob - belgrano</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -891,6 +891,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -971,7 +985,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1006,22 +1020,28 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1342,7 +1362,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A190BE11-27A5-497D-A254-ABC1C6ECE211}">
   <dimension ref="D6:Y28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G31" sqref="G31"/>
     </sheetView>
   </sheetViews>
@@ -1369,29 +1389,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:25" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="14"/>
-      <c r="L6" s="14"/>
-      <c r="M6" s="14"/>
-      <c r="N6" s="14"/>
-      <c r="O6" s="14"/>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
     </row>
     <row r="8" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
@@ -2840,13 +2860,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
+      <c r="F9" s="19"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
+      <c r="I9" s="19"/>
     </row>
     <row r="11" spans="5:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
@@ -3001,10 +3021,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2B0C72-7996-4F05-A4C8-44CF30165835}">
   <dimension ref="A9:AH114"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="B8" sqref="B8"/>
+      <selection pane="topRight" activeCell="M27" sqref="M27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3026,7 +3046,7 @@
     <col min="16" max="16" width="8.7109375" customWidth="1"/>
     <col min="17" max="17" width="27.7109375" customWidth="1"/>
     <col min="18" max="18" width="8.7109375" customWidth="1"/>
-    <col min="19" max="19" width="27.7109375" customWidth="1"/>
+    <col min="19" max="19" width="29.42578125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="8.7109375" customWidth="1"/>
     <col min="21" max="21" width="27.7109375" customWidth="1"/>
     <col min="24" max="24" width="33.5703125" bestFit="1" customWidth="1"/>
@@ -3034,43 +3054,43 @@
   <sheetData>
     <row r="9" spans="1:34" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C9" s="11" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="D9" s="11"/>
       <c r="E9" s="12" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F9" s="12"/>
       <c r="G9" s="12" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="H9" s="12"/>
       <c r="I9" s="12" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="J9" s="12"/>
       <c r="K9" s="12" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="L9" s="12"/>
       <c r="M9" s="12" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="N9" s="12"/>
       <c r="O9" s="12" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="P9" s="12"/>
       <c r="Q9" s="12" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="R9" s="12"/>
       <c r="S9" s="12" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="T9" s="12"/>
       <c r="U9" s="12" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3084,42 +3104,42 @@
         <v>30</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F10" s="10"/>
       <c r="G10" s="10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H10" s="10"/>
       <c r="I10" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="J10" s="10"/>
       <c r="K10" s="10" t="s">
-        <v>70</v>
+        <v>244</v>
       </c>
       <c r="L10" s="10"/>
       <c r="M10" s="10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="N10" s="10"/>
       <c r="O10" s="10" t="s">
-        <v>91</v>
+        <v>181</v>
       </c>
       <c r="P10" s="10"/>
       <c r="Q10" s="10" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="R10" s="10"/>
       <c r="S10" s="10" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="T10" s="10"/>
       <c r="U10" s="10" t="s">
-        <v>124</v>
+        <v>248</v>
       </c>
       <c r="AB10" s="8"/>
       <c r="AD10" s="8"/>
@@ -3135,43 +3155,43 @@
       <c r="C11" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="18" t="s">
-        <v>240</v>
+      <c r="D11" s="16" t="s">
+        <v>231</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="10" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H11" s="10"/>
       <c r="I11" s="10" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="J11" s="10"/>
       <c r="K11" s="10" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="L11" s="10"/>
       <c r="M11" s="10" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="N11" s="10"/>
       <c r="O11" s="10" t="s">
-        <v>92</v>
+        <v>182</v>
       </c>
       <c r="P11" s="10"/>
       <c r="Q11" s="10" t="s">
-        <v>103</v>
+        <v>246</v>
       </c>
       <c r="R11" s="10"/>
       <c r="S11" s="10" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="T11" s="10"/>
       <c r="U11" s="10" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="AH11" s="8"/>
     </row>
@@ -3186,42 +3206,42 @@
         <v>32</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="J12" s="10"/>
       <c r="K12" s="10" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="L12" s="10"/>
       <c r="M12" s="10" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="N12" s="10"/>
-      <c r="O12" s="10" t="s">
-        <v>93</v>
+      <c r="O12" s="20" t="s">
+        <v>183</v>
       </c>
       <c r="P12" s="10"/>
       <c r="Q12" s="10" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="R12" s="10"/>
       <c r="S12" s="10" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="T12" s="10"/>
       <c r="U12" s="10" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3235,42 +3255,42 @@
         <v>33</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F13" s="10"/>
       <c r="G13" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H13" s="10"/>
       <c r="I13" s="10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J13" s="10"/>
       <c r="K13" s="10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="L13" s="10"/>
       <c r="M13" s="10" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="10" t="s">
-        <v>94</v>
+        <v>184</v>
       </c>
       <c r="P13" s="10"/>
       <c r="Q13" s="10" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="R13" s="10"/>
       <c r="S13" s="10" t="s">
-        <v>116</v>
+        <v>247</v>
       </c>
       <c r="T13" s="10"/>
       <c r="U13" s="10" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3283,43 +3303,43 @@
       <c r="C14" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D14" s="19" t="s">
-        <v>243</v>
+      <c r="D14" s="17" t="s">
+        <v>234</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H14" s="10"/>
       <c r="I14" s="10" t="s">
-        <v>64</v>
+        <v>243</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L14" s="10"/>
       <c r="M14" s="10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="10" t="s">
-        <v>95</v>
+        <v>185</v>
       </c>
       <c r="P14" s="10"/>
       <c r="Q14" s="10" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="R14" s="10"/>
       <c r="S14" s="10" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="T14" s="10"/>
       <c r="U14" s="10" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3330,45 +3350,45 @@
         <v>5</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>35</v>
+        <v>240</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F15" s="10"/>
       <c r="G15" s="10" t="s">
-        <v>55</v>
+        <v>242</v>
       </c>
       <c r="H15" s="10"/>
       <c r="I15" s="10" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="J15" s="10"/>
       <c r="K15" s="10" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="L15" s="10"/>
       <c r="M15" s="10" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10" t="s">
-        <v>96</v>
+        <v>186</v>
       </c>
       <c r="P15" s="10"/>
       <c r="Q15" s="10" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="R15" s="10"/>
       <c r="S15" s="10" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="T15" s="10"/>
       <c r="U15" s="10" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:34" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3379,45 +3399,45 @@
         <v>6</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F16" s="10"/>
       <c r="G16" s="10" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="H16" s="10"/>
       <c r="I16" s="10" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="J16" s="10"/>
       <c r="K16" s="10" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="L16" s="10"/>
       <c r="M16" s="10" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10" t="s">
-        <v>97</v>
+        <v>187</v>
       </c>
       <c r="P16" s="10"/>
       <c r="Q16" s="10" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="R16" s="10"/>
       <c r="S16" s="10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="T16" s="10"/>
       <c r="U16" s="10" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3428,45 +3448,45 @@
         <v>21</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>47</v>
+        <v>241</v>
       </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="H17" s="10"/>
       <c r="I17" s="10" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="J17" s="10"/>
       <c r="K17" s="10" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="L17" s="10"/>
       <c r="M17" s="10" t="s">
-        <v>87</v>
+        <v>245</v>
       </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10" t="s">
-        <v>98</v>
+        <v>188</v>
       </c>
       <c r="P17" s="10"/>
       <c r="Q17" s="10" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="R17" s="10"/>
       <c r="S17" s="10" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="T17" s="10"/>
       <c r="U17" s="10" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3477,45 +3497,45 @@
         <v>7</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="H18" s="10"/>
       <c r="I18" s="10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="J18" s="10"/>
       <c r="K18" s="10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="L18" s="10"/>
       <c r="M18" s="10" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="N18" s="10"/>
       <c r="O18" s="10" t="s">
-        <v>99</v>
+        <v>189</v>
       </c>
       <c r="P18" s="10"/>
       <c r="Q18" s="10" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="R18" s="10"/>
       <c r="S18" s="10" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="T18" s="10"/>
       <c r="U18" s="10" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3526,45 +3546,45 @@
         <v>8</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F19" s="10"/>
       <c r="G19" s="10" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="H19" s="10"/>
       <c r="I19" s="10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="J19" s="10"/>
       <c r="K19" s="10" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="L19" s="10"/>
       <c r="M19" s="10" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="N19" s="10"/>
       <c r="O19" s="10" t="s">
-        <v>100</v>
+        <v>190</v>
       </c>
       <c r="P19" s="10"/>
       <c r="Q19" s="10" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="R19" s="10"/>
       <c r="S19" s="10" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="T19" s="10"/>
       <c r="U19" s="10" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3602,41 +3622,41 @@
         <v>10</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D21" s="11"/>
       <c r="E21" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F21" s="11"/>
       <c r="G21" s="11" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="H21" s="11"/>
       <c r="I21" s="11" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="J21" s="11"/>
       <c r="K21" s="11" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="L21" s="11"/>
       <c r="M21" s="11" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="N21" s="11"/>
       <c r="O21" s="11" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="P21" s="11"/>
       <c r="Q21" s="11" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="R21" s="11"/>
       <c r="S21" s="11" t="s">
-        <v>222</v>
-      </c>
-      <c r="T21" s="16"/>
+        <v>213</v>
+      </c>
+      <c r="T21" s="14"/>
       <c r="U21" s="9"/>
     </row>
     <row r="22" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3647,41 +3667,41 @@
         <v>11</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F22" s="10"/>
       <c r="G22" s="10" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="H22" s="10"/>
       <c r="I22" s="10" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="J22" s="10"/>
       <c r="K22" s="10" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="L22" s="10"/>
       <c r="M22" s="10" t="s">
-        <v>190</v>
+        <v>85</v>
       </c>
       <c r="N22" s="10"/>
       <c r="O22" s="10" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="P22" s="10"/>
       <c r="Q22" s="10" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="R22" s="10"/>
       <c r="S22" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="T22" s="17"/>
+        <v>214</v>
+      </c>
+      <c r="T22" s="15"/>
       <c r="U22" s="9"/>
     </row>
     <row r="23" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3692,41 +3712,41 @@
         <v>12</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="D23" s="10"/>
       <c r="E23" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F23" s="10"/>
       <c r="G23" s="10" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="H23" s="10"/>
       <c r="I23" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="J23" s="10"/>
       <c r="K23" s="10" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="L23" s="10"/>
       <c r="M23" s="10" t="s">
-        <v>191</v>
+        <v>86</v>
       </c>
       <c r="N23" s="10"/>
       <c r="O23" s="10" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="P23" s="10"/>
       <c r="Q23" s="10" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="R23" s="10"/>
       <c r="S23" s="10" t="s">
-        <v>224</v>
-      </c>
-      <c r="T23" s="17"/>
+        <v>215</v>
+      </c>
+      <c r="T23" s="15"/>
       <c r="U23" s="9"/>
     </row>
     <row r="24" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3737,41 +3757,41 @@
         <v>13</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="D24" s="10"/>
       <c r="E24" s="10" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="F24" s="10"/>
       <c r="G24" s="10" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="H24" s="10"/>
       <c r="I24" s="10" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="J24" s="10"/>
       <c r="K24" s="10" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="L24" s="10"/>
       <c r="M24" s="10" t="s">
-        <v>192</v>
+        <v>87</v>
       </c>
       <c r="N24" s="10"/>
       <c r="O24" s="10" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="P24" s="10"/>
       <c r="Q24" s="10" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="R24" s="10"/>
       <c r="S24" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="T24" s="17"/>
+        <v>216</v>
+      </c>
+      <c r="T24" s="15"/>
       <c r="U24" s="13"/>
     </row>
     <row r="25" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3782,41 +3802,41 @@
         <v>14</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="D25" s="10"/>
       <c r="E25" s="10" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F25" s="10"/>
       <c r="G25" s="10" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="H25" s="10"/>
       <c r="I25" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="J25" s="10"/>
       <c r="K25" s="10" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="L25" s="10"/>
       <c r="M25" s="10" t="s">
-        <v>193</v>
+        <v>88</v>
       </c>
       <c r="N25" s="10"/>
       <c r="O25" s="10" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="P25" s="10"/>
       <c r="Q25" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="R25" s="10"/>
       <c r="S25" s="10" t="s">
-        <v>226</v>
-      </c>
-      <c r="T25" s="17"/>
+        <v>217</v>
+      </c>
+      <c r="T25" s="15"/>
       <c r="U25" s="9"/>
     </row>
     <row r="26" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3827,41 +3847,41 @@
         <v>15</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D26" s="10"/>
       <c r="E26" s="10" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="F26" s="10"/>
       <c r="G26" s="10" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="H26" s="10"/>
       <c r="I26" s="10" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="J26" s="10"/>
       <c r="K26" s="10" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="L26" s="10"/>
       <c r="M26" s="10" t="s">
-        <v>194</v>
+        <v>89</v>
       </c>
       <c r="N26" s="10"/>
       <c r="O26" s="10" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="P26" s="10"/>
       <c r="Q26" s="10" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="R26" s="10"/>
       <c r="S26" s="10" t="s">
-        <v>227</v>
-      </c>
-      <c r="T26" s="17"/>
+        <v>218</v>
+      </c>
+      <c r="T26" s="15"/>
       <c r="U26" s="9"/>
     </row>
     <row r="27" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3872,41 +3892,41 @@
         <v>16</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="D27" s="10"/>
       <c r="E27" s="10" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="H27" s="10"/>
       <c r="I27" s="10" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="J27" s="10"/>
       <c r="K27" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="L27" s="10"/>
-      <c r="M27" s="10" t="s">
-        <v>195</v>
+      <c r="M27" s="21" t="s">
+        <v>90</v>
       </c>
       <c r="N27" s="10"/>
       <c r="O27" s="10" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="P27" s="10"/>
       <c r="Q27" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="R27" s="10"/>
       <c r="S27" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="T27" s="17"/>
+        <v>219</v>
+      </c>
+      <c r="T27" s="15"/>
       <c r="U27" s="9"/>
     </row>
     <row r="28" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3917,41 +3937,41 @@
         <v>17</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D28" s="10"/>
       <c r="E28" s="10" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="F28" s="10"/>
       <c r="G28" s="10" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="H28" s="10"/>
       <c r="I28" s="10" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="J28" s="10"/>
       <c r="K28" s="10" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="L28" s="10"/>
       <c r="M28" s="10" t="s">
-        <v>196</v>
+        <v>91</v>
       </c>
       <c r="N28" s="10"/>
       <c r="O28" s="10" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="P28" s="10"/>
       <c r="Q28" s="10" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="10" t="s">
-        <v>229</v>
-      </c>
-      <c r="T28" s="17"/>
+        <v>220</v>
+      </c>
+      <c r="T28" s="15"/>
       <c r="U28" s="9"/>
     </row>
     <row r="29" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
@@ -3962,119 +3982,119 @@
         <v>18</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="D29" s="10"/>
       <c r="E29" s="10" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F29" s="10"/>
       <c r="G29" s="10" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="H29" s="10"/>
       <c r="I29" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="J29" s="10"/>
       <c r="K29" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="L29" s="10"/>
       <c r="M29" s="10" t="s">
-        <v>197</v>
+        <v>92</v>
       </c>
       <c r="N29" s="10"/>
       <c r="O29" s="10" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="P29" s="10"/>
       <c r="Q29" s="10" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="R29" s="10"/>
       <c r="S29" s="10" t="s">
-        <v>230</v>
-      </c>
-      <c r="T29" s="17"/>
+        <v>221</v>
+      </c>
+      <c r="T29" s="15"/>
       <c r="U29" s="9"/>
     </row>
     <row r="30" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C30" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D30" s="10"/>
       <c r="E30" s="10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F30" s="10"/>
       <c r="G30" s="10" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="H30" s="10"/>
       <c r="I30" s="10" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="J30" s="10"/>
       <c r="K30" s="10" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="L30" s="10"/>
       <c r="M30" s="10" t="s">
-        <v>198</v>
+        <v>93</v>
       </c>
       <c r="N30" s="10"/>
       <c r="O30" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="P30" s="10"/>
       <c r="Q30" s="10" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="R30" s="10"/>
       <c r="S30" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="T30" s="17"/>
+        <v>222</v>
+      </c>
+      <c r="T30" s="15"/>
       <c r="U30" s="9"/>
     </row>
     <row r="31" spans="1:21" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C31" s="10" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="D31" s="10"/>
       <c r="E31" s="10" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="H31" s="10"/>
       <c r="I31" s="10" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="J31" s="10"/>
       <c r="K31" s="10" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="L31" s="10"/>
       <c r="M31" s="10" t="s">
-        <v>199</v>
+        <v>94</v>
       </c>
       <c r="N31" s="10"/>
       <c r="O31" s="10" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="P31" s="10"/>
       <c r="Q31" s="10" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="R31" s="10"/>
       <c r="S31" s="10" t="s">
-        <v>232</v>
-      </c>
-      <c r="T31" s="17"/>
+        <v>223</v>
+      </c>
+      <c r="T31" s="15"/>
       <c r="U31" s="9"/>
     </row>
     <row r="114" spans="21:21" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
se subio algo de la presentacion
</commit_message>
<xml_diff>
--- a/MaterialUtil/MatrizDistancias.xlsx
+++ b/MaterialUtil/MatrizDistancias.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Colo\TUP\Matematicas\Trabajo Practico\TP_Matematica\MaterialUtil\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucio\Desktop\Programacion\1er Cuatrimestre\Matematicas\TPGrafos\TP_Matematica\MaterialUtil\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B58EE49-7FD7-48EB-BE29-DED513AEE1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F26EF5-6CED-4040-B5BC-AA1D040D7341}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="2" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8E2A5D20-47A1-4900-A7A2-031089E38D2A}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -906,7 +906,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -926,6 +926,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -985,7 +1003,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1032,16 +1050,34 @@
     <xf numFmtId="17" fontId="10" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1362,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A190BE11-27A5-497D-A254-ABC1C6ECE211}">
   <dimension ref="D6:Y28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+    <sheetView topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="Y16" activeCellId="2" sqref="G16 X16 Y16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,29 +1425,29 @@
   </cols>
   <sheetData>
     <row r="6" spans="4:25" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="18"/>
-      <c r="Q6" s="18"/>
-      <c r="R6" s="18"/>
-      <c r="S6" s="18"/>
-      <c r="T6" s="18"/>
-      <c r="U6" s="18"/>
-      <c r="V6" s="18"/>
-      <c r="W6" s="18"/>
-      <c r="X6" s="18"/>
-      <c r="Y6" s="18"/>
+      <c r="F6" s="20"/>
+      <c r="G6" s="20"/>
+      <c r="H6" s="20"/>
+      <c r="I6" s="20"/>
+      <c r="J6" s="20"/>
+      <c r="K6" s="20"/>
+      <c r="L6" s="20"/>
+      <c r="M6" s="20"/>
+      <c r="N6" s="20"/>
+      <c r="O6" s="20"/>
+      <c r="P6" s="20"/>
+      <c r="Q6" s="20"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="20"/>
+      <c r="T6" s="20"/>
+      <c r="U6" s="20"/>
+      <c r="V6" s="20"/>
+      <c r="W6" s="20"/>
+      <c r="X6" s="20"/>
+      <c r="Y6" s="20"/>
     </row>
     <row r="8" spans="4:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E8" s="1"/>
@@ -1891,7 +1927,7 @@
       <c r="E15" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15" s="26">
         <v>313</v>
       </c>
       <c r="G15" s="3">
@@ -1903,10 +1939,10 @@
       <c r="I15" s="3">
         <v>317</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="22">
         <v>316</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="26">
         <v>320</v>
       </c>
       <c r="L15" s="3">
@@ -1915,7 +1951,7 @@
       <c r="M15" s="3">
         <v>7</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="26">
         <v>366</v>
       </c>
       <c r="O15" s="3">
@@ -1933,13 +1969,13 @@
       <c r="S15" s="3">
         <v>165</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15" s="22">
         <v>323</v>
       </c>
       <c r="U15" s="3">
         <v>322</v>
       </c>
-      <c r="V15" s="3">
+      <c r="V15" s="22">
         <v>304</v>
       </c>
       <c r="W15" s="3">
@@ -1962,7 +1998,7 @@
       <c r="F16" s="3">
         <v>287</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="26">
         <v>304</v>
       </c>
       <c r="H16" s="3">
@@ -1971,10 +2007,10 @@
       <c r="I16" s="3">
         <v>305</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="25">
         <v>305</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="22">
         <v>309</v>
       </c>
       <c r="L16" s="3">
@@ -1995,13 +2031,13 @@
       <c r="Q16" s="3">
         <v>405</v>
       </c>
-      <c r="R16" s="3">
+      <c r="R16" s="22">
         <v>175</v>
       </c>
       <c r="S16" s="3">
         <v>173</v>
       </c>
-      <c r="T16" s="3">
+      <c r="T16" s="22">
         <v>312</v>
       </c>
       <c r="U16" s="3">
@@ -2013,10 +2049,10 @@
       <c r="W16" s="3">
         <v>292</v>
       </c>
-      <c r="X16" s="3">
+      <c r="X16" s="26">
         <v>278</v>
       </c>
-      <c r="Y16" s="3">
+      <c r="Y16" s="26">
         <v>284</v>
       </c>
     </row>
@@ -2860,13 +2896,13 @@
   </cols>
   <sheetData>
     <row r="9" spans="5:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="E9" s="19" t="s">
+      <c r="E9" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
     </row>
     <row r="11" spans="5:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="E11" s="5" t="s">
@@ -3021,10 +3057,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF2B0C72-7996-4F05-A4C8-44CF30165835}">
   <dimension ref="A9:AH114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="F1" activePane="topRight" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="K1" activePane="topRight" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="topRight" activeCell="M27" sqref="M27"/>
+      <selection pane="topRight" activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3118,7 +3154,7 @@
         <v>57</v>
       </c>
       <c r="J10" s="10"/>
-      <c r="K10" s="10" t="s">
+      <c r="K10" s="27" t="s">
         <v>244</v>
       </c>
       <c r="L10" s="10"/>
@@ -3174,7 +3210,7 @@
         <v>66</v>
       </c>
       <c r="L11" s="10"/>
-      <c r="M11" s="10" t="s">
+      <c r="M11" s="27" t="s">
         <v>76</v>
       </c>
       <c r="N11" s="10"/>
@@ -3228,7 +3264,7 @@
         <v>77</v>
       </c>
       <c r="N12" s="10"/>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="18" t="s">
         <v>183</v>
       </c>
       <c r="P12" s="10"/>
@@ -3261,7 +3297,7 @@
         <v>42</v>
       </c>
       <c r="F13" s="10"/>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="23" t="s">
         <v>51</v>
       </c>
       <c r="H13" s="10"/>
@@ -3314,7 +3350,7 @@
         <v>52</v>
       </c>
       <c r="H14" s="10"/>
-      <c r="I14" s="10" t="s">
+      <c r="I14" s="23" t="s">
         <v>243</v>
       </c>
       <c r="J14" s="10"/>
@@ -3349,7 +3385,7 @@
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="24" t="s">
         <v>240</v>
       </c>
       <c r="D15" s="10" t="s">
@@ -3359,7 +3395,7 @@
         <v>44</v>
       </c>
       <c r="F15" s="10"/>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="27" t="s">
         <v>242</v>
       </c>
       <c r="H15" s="10"/>
@@ -3404,7 +3440,7 @@
       <c r="D16" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="27" t="s">
         <v>45</v>
       </c>
       <c r="F16" s="10"/>
@@ -3416,7 +3452,7 @@
         <v>62</v>
       </c>
       <c r="J16" s="10"/>
-      <c r="K16" s="10" t="s">
+      <c r="K16" s="23" t="s">
         <v>71</v>
       </c>
       <c r="L16" s="10"/>
@@ -3447,13 +3483,13 @@
       <c r="B17" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="23" t="s">
         <v>36</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="23" t="s">
         <v>241</v>
       </c>
       <c r="F17" s="10"/>
@@ -3461,7 +3497,7 @@
         <v>54</v>
       </c>
       <c r="H17" s="10"/>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="27" t="s">
         <v>63</v>
       </c>
       <c r="J17" s="10"/>
@@ -3469,7 +3505,7 @@
         <v>72</v>
       </c>
       <c r="L17" s="10"/>
-      <c r="M17" s="10" t="s">
+      <c r="M17" s="23" t="s">
         <v>245</v>
       </c>
       <c r="N17" s="10"/>
@@ -3911,7 +3947,7 @@
         <v>175</v>
       </c>
       <c r="L27" s="10"/>
-      <c r="M27" s="21" t="s">
+      <c r="M27" s="19" t="s">
         <v>90</v>
       </c>
       <c r="N27" s="10"/>

</xml_diff>